<commit_message>
export timeseries functions to excel (60/1114)
</commit_message>
<xml_diff>
--- a/UnitTests/Tests/Date.xlsx
+++ b/UnitTests/Tests/Date.xlsx
@@ -1126,15 +1126,15 @@
         <v>25569</v>
       </c>
       <c r="C30">
-        <v>38371</v>
+        <v>25569</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E30">
         <f>_xll.qlECBKnownDates()</f>
-        <v>38371</v>
+        <v>25569</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1300,15 +1300,15 @@
         <v>1</v>
       </c>
       <c r="C39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E39" t="b">
         <f>_xll.qlECBIsECBdate(25569)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
export index functions to excel (92/1114)
</commit_message>
<xml_diff>
--- a/UnitTests/Tests/Date.xlsx
+++ b/UnitTests/Tests/Date.xlsx
@@ -1126,15 +1126,15 @@
         <v>38371</v>
       </c>
       <c r="C30">
-        <v>38371</v>
+        <v>25569</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="E30">
         <f>_xll.qlECBKnownDates()</f>
-        <v>38371</v>
+        <v>25569</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1300,15 +1300,15 @@
         <v>1</v>
       </c>
       <c r="C39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E39" t="b">
         <f>_xll.qlECBIsECBdate(25569)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
set eval date for unit tests
</commit_message>
<xml_diff>
--- a/UnitTests/Tests/Date.xlsx
+++ b/UnitTests/Tests/Date.xlsx
@@ -864,7 +864,7 @@
         <v>PASS</v>
       </c>
       <c r="E16" t="str">
-        <f>_xll.qlIMMCode(42081)</f>
+        <f>_xll.qlIMMcode(42081)</f>
         <v>H5</v>
       </c>
       <c r="G16" s="5">
@@ -924,7 +924,7 @@
         <v>PASS</v>
       </c>
       <c r="E19">
-        <f>_xll.qlIMMDate("H5")</f>
+        <f>_xll.qlIMMdate("H5")</f>
         <v>45735</v>
       </c>
     </row>
@@ -1019,7 +1019,7 @@
         <v>PASS</v>
       </c>
       <c r="E24" t="str">
-        <f>_xll.qlASXCode(42713)</f>
+        <f>_xll.qlASXcode(42713)</f>
         <v>Z6</v>
       </c>
     </row>
@@ -1076,7 +1076,7 @@
         <v>PASS</v>
       </c>
       <c r="E27">
-        <f>_xll.qlASXDate("H5")</f>
+        <f>_xll.qlASXdate("H5")</f>
         <v>45730</v>
       </c>
     </row>
@@ -1123,14 +1123,14 @@
         <v>35</v>
       </c>
       <c r="B30">
-        <v>38371</v>
+        <v>25569</v>
       </c>
       <c r="C30">
         <v>25569</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E30">
         <f>_xll.qlECBKnownDates()</f>
@@ -1190,7 +1190,7 @@
         <v>PASS</v>
       </c>
       <c r="E33">
-        <f>_xll.qlECBDate2("january",1971)</f>
+        <f>_xll.qlECBdate2("january",1971)</f>
         <v>38371</v>
       </c>
     </row>
@@ -1209,7 +1209,7 @@
         <v>PASS</v>
       </c>
       <c r="E34">
-        <f>_xll.qlECBDate("MAR10")</f>
+        <f>_xll.qlECBdate("MAR10")</f>
         <v>40247</v>
       </c>
     </row>
@@ -1228,7 +1228,7 @@
         <v>PASS</v>
       </c>
       <c r="E35" t="str">
-        <f>_xll.qlECBCode(40247)</f>
+        <f>_xll.qlECBcode(40247)</f>
         <v>MAR10</v>
       </c>
       <c r="G35" s="5">
@@ -1297,14 +1297,14 @@
         <v>44</v>
       </c>
       <c r="B39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39" t="b">
         <v>1</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E39" t="b">
         <f>_xll.qlECBIsECBdate(25569)</f>

</xml_diff>